<commit_message>
read single is tested
</commit_message>
<xml_diff>
--- a/devices/exam_config.xlsx
+++ b/devices/exam_config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>ip</t>
   </si>
@@ -467,6 +467,26 @@
         <scheme val="minor"/>
       </rPr>
       <t>optionaly</t>
+    </r>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNIT-ID (1-127) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
     </r>
   </si>
 </sst>
@@ -1367,31 +1387,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16" style="4" customWidth="1"/>
-    <col min="8" max="8" width="17" style="4" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="25" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" style="4" customWidth="1"/>
+    <col min="3" max="4" width="22.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="25" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="25.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1402,40 +1422,43 @@
         <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1446,40 +1469,43 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1490,40 +1516,43 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>19003</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4">
         <v>1</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1534,40 +1563,43 @@
         <v>3</v>
       </c>
       <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>19001</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1578,36 +1610,39 @@
         <v>3</v>
       </c>
       <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
         <v>5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>19002</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
       </c>
       <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4">
         <v>1</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>